<commit_message>
Fix data-driven test: using GlobalVariable
</commit_message>
<xml_diff>
--- a/Data Files/Accounts.xlsx
+++ b/Data Files/Accounts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A93D14-A96D-BE4C-9120-22424B9D7732}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F5B71-6A27-B246-A524-28F5C77A6326}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_accounts" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -520,9 +520,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DAF65FE4-A399-F845-94FB-39172FC7DAB1}"/>

</xml_diff>